<commit_message>
feat: take review changes, improve and add regex, add changelog,
</commit_message>
<xml_diff>
--- a/SchemaDispositifAide.xlsx
+++ b/SchemaDispositifAide.xlsx
@@ -481,7 +481,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
-Exemple : DEP01|COM83141
+Exemple : DEP-01|COM-83141
 </t>
     </r>
   </si>
@@ -542,7 +542,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -609,13 +609,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -742,7 +735,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -803,15 +796,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1083,8 +1072,8 @@
   </sheetPr>
   <dimension ref="A1:XFD1010"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1102,7 +1091,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16346" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16346" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,7 +1236,7 @@
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" s="16" customFormat="true" ht="22.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
@@ -1287,56 +1276,56 @@
       <c r="M9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="15" t="s">
+      <c r="N9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="15" t="s">
+      <c r="O9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="15" t="s">
+      <c r="P9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="XDR9" s="0"/>
-      <c r="XDS9" s="0"/>
-      <c r="XDT9" s="0"/>
-      <c r="XDU9" s="0"/>
-      <c r="XDV9" s="0"/>
-      <c r="XDW9" s="0"/>
-      <c r="XDX9" s="0"/>
-      <c r="XDY9" s="0"/>
-      <c r="XDZ9" s="0"/>
-      <c r="XEA9" s="0"/>
-      <c r="XEB9" s="0"/>
-      <c r="XEC9" s="0"/>
-      <c r="XED9" s="0"/>
-      <c r="XEE9" s="0"/>
-      <c r="XEF9" s="0"/>
-      <c r="XEG9" s="0"/>
-      <c r="XEH9" s="0"/>
-      <c r="XEI9" s="0"/>
-      <c r="XEJ9" s="0"/>
-      <c r="XEK9" s="0"/>
-      <c r="XEL9" s="0"/>
-      <c r="XEM9" s="0"/>
-      <c r="XEN9" s="0"/>
-      <c r="XEO9" s="0"/>
-      <c r="XEP9" s="0"/>
-      <c r="XEQ9" s="0"/>
-      <c r="XER9" s="0"/>
-      <c r="XES9" s="0"/>
-      <c r="XET9" s="0"/>
-      <c r="XEU9" s="0"/>
-      <c r="XEV9" s="0"/>
-      <c r="XEW9" s="0"/>
-      <c r="XEX9" s="0"/>
-      <c r="XEY9" s="0"/>
-      <c r="XEZ9" s="0"/>
-      <c r="XFA9" s="0"/>
-      <c r="XFB9" s="0"/>
-      <c r="XFC9" s="0"/>
-      <c r="XFD9" s="0"/>
-    </row>
-    <row r="10" s="17" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XDR9" s="1"/>
+      <c r="XDS9" s="1"/>
+      <c r="XDT9" s="1"/>
+      <c r="XDU9" s="1"/>
+      <c r="XDV9" s="1"/>
+      <c r="XDW9" s="1"/>
+      <c r="XDX9" s="1"/>
+      <c r="XDY9" s="1"/>
+      <c r="XDZ9" s="1"/>
+      <c r="XEA9" s="1"/>
+      <c r="XEB9" s="1"/>
+      <c r="XEC9" s="1"/>
+      <c r="XED9" s="1"/>
+      <c r="XEE9" s="1"/>
+      <c r="XEF9" s="1"/>
+      <c r="XEG9" s="1"/>
+      <c r="XEH9" s="1"/>
+      <c r="XEI9" s="1"/>
+      <c r="XEJ9" s="1"/>
+      <c r="XEK9" s="1"/>
+      <c r="XEL9" s="1"/>
+      <c r="XEM9" s="1"/>
+      <c r="XEN9" s="1"/>
+      <c r="XEO9" s="1"/>
+      <c r="XEP9" s="1"/>
+      <c r="XEQ9" s="1"/>
+      <c r="XER9" s="1"/>
+      <c r="XES9" s="1"/>
+      <c r="XET9" s="1"/>
+      <c r="XEU9" s="1"/>
+      <c r="XEV9" s="1"/>
+      <c r="XEW9" s="1"/>
+      <c r="XEX9" s="1"/>
+      <c r="XEY9" s="1"/>
+      <c r="XEZ9" s="1"/>
+      <c r="XFA9" s="1"/>
+      <c r="XFB9" s="1"/>
+      <c r="XFC9" s="1"/>
+      <c r="XFD9" s="1"/>
+    </row>
+    <row r="10" s="16" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1376,7 +1365,7 @@
       <c r="M10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="15" t="s">
+      <c r="N10" s="14" t="s">
         <v>34</v>
       </c>
       <c r="O10" s="14" t="s">
@@ -1385,47 +1374,47 @@
       <c r="P10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="XDR10" s="0"/>
-      <c r="XDS10" s="0"/>
-      <c r="XDT10" s="0"/>
-      <c r="XDU10" s="0"/>
-      <c r="XDV10" s="0"/>
-      <c r="XDW10" s="0"/>
-      <c r="XDX10" s="0"/>
-      <c r="XDY10" s="0"/>
-      <c r="XDZ10" s="0"/>
-      <c r="XEA10" s="0"/>
-      <c r="XEB10" s="0"/>
-      <c r="XEC10" s="0"/>
-      <c r="XED10" s="0"/>
-      <c r="XEE10" s="0"/>
-      <c r="XEF10" s="0"/>
-      <c r="XEG10" s="0"/>
-      <c r="XEH10" s="0"/>
-      <c r="XEI10" s="0"/>
-      <c r="XEJ10" s="0"/>
-      <c r="XEK10" s="0"/>
-      <c r="XEL10" s="0"/>
-      <c r="XEM10" s="0"/>
-      <c r="XEN10" s="0"/>
-      <c r="XEO10" s="0"/>
-      <c r="XEP10" s="0"/>
-      <c r="XEQ10" s="0"/>
-      <c r="XER10" s="0"/>
-      <c r="XES10" s="0"/>
-      <c r="XET10" s="0"/>
-      <c r="XEU10" s="0"/>
-      <c r="XEV10" s="0"/>
-      <c r="XEW10" s="0"/>
-      <c r="XEX10" s="0"/>
-      <c r="XEY10" s="0"/>
-      <c r="XEZ10" s="0"/>
-      <c r="XFA10" s="0"/>
-      <c r="XFB10" s="0"/>
-      <c r="XFC10" s="0"/>
-      <c r="XFD10" s="0"/>
-    </row>
-    <row r="11" s="16" customFormat="true" ht="431.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="XDR10" s="1"/>
+      <c r="XDS10" s="1"/>
+      <c r="XDT10" s="1"/>
+      <c r="XDU10" s="1"/>
+      <c r="XDV10" s="1"/>
+      <c r="XDW10" s="1"/>
+      <c r="XDX10" s="1"/>
+      <c r="XDY10" s="1"/>
+      <c r="XDZ10" s="1"/>
+      <c r="XEA10" s="1"/>
+      <c r="XEB10" s="1"/>
+      <c r="XEC10" s="1"/>
+      <c r="XED10" s="1"/>
+      <c r="XEE10" s="1"/>
+      <c r="XEF10" s="1"/>
+      <c r="XEG10" s="1"/>
+      <c r="XEH10" s="1"/>
+      <c r="XEI10" s="1"/>
+      <c r="XEJ10" s="1"/>
+      <c r="XEK10" s="1"/>
+      <c r="XEL10" s="1"/>
+      <c r="XEM10" s="1"/>
+      <c r="XEN10" s="1"/>
+      <c r="XEO10" s="1"/>
+      <c r="XEP10" s="1"/>
+      <c r="XEQ10" s="1"/>
+      <c r="XER10" s="1"/>
+      <c r="XES10" s="1"/>
+      <c r="XET10" s="1"/>
+      <c r="XEU10" s="1"/>
+      <c r="XEV10" s="1"/>
+      <c r="XEW10" s="1"/>
+      <c r="XEX10" s="1"/>
+      <c r="XEY10" s="1"/>
+      <c r="XEZ10" s="1"/>
+      <c r="XFA10" s="1"/>
+      <c r="XFB10" s="1"/>
+      <c r="XFC10" s="1"/>
+      <c r="XFD10" s="1"/>
+    </row>
+    <row r="11" s="15" customFormat="true" ht="431.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
         <v>37</v>
       </c>
@@ -1447,16 +1436,16 @@
       <c r="G11" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="17" t="s">
         <v>47</v>
       </c>
       <c r="L11" s="13" t="s">
@@ -1465,57 +1454,57 @@
       <c r="M11" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="P11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="XDR11" s="0"/>
-      <c r="XDS11" s="0"/>
-      <c r="XDT11" s="0"/>
-      <c r="XDU11" s="0"/>
-      <c r="XDV11" s="0"/>
-      <c r="XDW11" s="0"/>
-      <c r="XDX11" s="0"/>
-      <c r="XDY11" s="0"/>
-      <c r="XDZ11" s="0"/>
-      <c r="XEA11" s="0"/>
-      <c r="XEB11" s="0"/>
-      <c r="XEC11" s="0"/>
-      <c r="XED11" s="0"/>
-      <c r="XEE11" s="0"/>
-      <c r="XEF11" s="0"/>
-      <c r="XEG11" s="0"/>
-      <c r="XEH11" s="0"/>
-      <c r="XEI11" s="0"/>
-      <c r="XEJ11" s="0"/>
-      <c r="XEK11" s="0"/>
-      <c r="XEL11" s="0"/>
-      <c r="XEM11" s="0"/>
-      <c r="XEN11" s="0"/>
-      <c r="XEO11" s="0"/>
-      <c r="XEP11" s="0"/>
-      <c r="XEQ11" s="0"/>
-      <c r="XER11" s="0"/>
-      <c r="XES11" s="0"/>
-      <c r="XET11" s="0"/>
-      <c r="XEU11" s="0"/>
-      <c r="XEV11" s="0"/>
-      <c r="XEW11" s="0"/>
-      <c r="XEX11" s="0"/>
-      <c r="XEY11" s="0"/>
-      <c r="XEZ11" s="0"/>
-      <c r="XFA11" s="0"/>
-      <c r="XFB11" s="0"/>
-      <c r="XFC11" s="0"/>
-      <c r="XFD11" s="0"/>
+      <c r="XDR11" s="1"/>
+      <c r="XDS11" s="1"/>
+      <c r="XDT11" s="1"/>
+      <c r="XDU11" s="1"/>
+      <c r="XDV11" s="1"/>
+      <c r="XDW11" s="1"/>
+      <c r="XDX11" s="1"/>
+      <c r="XDY11" s="1"/>
+      <c r="XDZ11" s="1"/>
+      <c r="XEA11" s="1"/>
+      <c r="XEB11" s="1"/>
+      <c r="XEC11" s="1"/>
+      <c r="XED11" s="1"/>
+      <c r="XEE11" s="1"/>
+      <c r="XEF11" s="1"/>
+      <c r="XEG11" s="1"/>
+      <c r="XEH11" s="1"/>
+      <c r="XEI11" s="1"/>
+      <c r="XEJ11" s="1"/>
+      <c r="XEK11" s="1"/>
+      <c r="XEL11" s="1"/>
+      <c r="XEM11" s="1"/>
+      <c r="XEN11" s="1"/>
+      <c r="XEO11" s="1"/>
+      <c r="XEP11" s="1"/>
+      <c r="XEQ11" s="1"/>
+      <c r="XER11" s="1"/>
+      <c r="XES11" s="1"/>
+      <c r="XET11" s="1"/>
+      <c r="XEU11" s="1"/>
+      <c r="XEV11" s="1"/>
+      <c r="XEW11" s="1"/>
+      <c r="XEX11" s="1"/>
+      <c r="XEY11" s="1"/>
+      <c r="XEZ11" s="1"/>
+      <c r="XFA11" s="1"/>
+      <c r="XFB11" s="1"/>
+      <c r="XFC11" s="1"/>
+      <c r="XFD11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="n">
+      <c r="A12" s="18" t="n">
         <v>1</v>
       </c>
       <c r="B12" s="3"/>
@@ -1535,12 +1524,12 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="n">
+      <c r="A13" s="18" t="n">
         <v>2</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="20"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1555,7 +1544,7 @@
       <c r="P13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="n">
+      <c r="A14" s="18" t="n">
         <v>3</v>
       </c>
       <c r="B14" s="3"/>
@@ -1575,7 +1564,7 @@
       <c r="P14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="n">
+      <c r="A15" s="18" t="n">
         <v>4</v>
       </c>
       <c r="B15" s="3"/>
@@ -1595,7 +1584,7 @@
       <c r="P15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="n">
+      <c r="A16" s="18" t="n">
         <v>5</v>
       </c>
       <c r="B16" s="3"/>
@@ -1615,7 +1604,7 @@
       <c r="P16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19" t="n">
+      <c r="A17" s="18" t="n">
         <v>6</v>
       </c>
       <c r="B17" s="3"/>
@@ -1635,7 +1624,7 @@
       <c r="P17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="n">
+      <c r="A18" s="18" t="n">
         <v>7</v>
       </c>
       <c r="B18" s="3"/>
@@ -1655,7 +1644,7 @@
       <c r="P18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19" t="n">
+      <c r="A19" s="18" t="n">
         <v>8</v>
       </c>
       <c r="B19" s="3"/>
@@ -1675,7 +1664,7 @@
       <c r="P19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19" t="n">
+      <c r="A20" s="18" t="n">
         <v>9</v>
       </c>
       <c r="B20" s="3"/>
@@ -1695,7 +1684,7 @@
       <c r="P20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="n">
+      <c r="A21" s="18" t="n">
         <v>10</v>
       </c>
       <c r="B21" s="3"/>
@@ -1715,7 +1704,7 @@
       <c r="P21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19" t="n">
+      <c r="A22" s="18" t="n">
         <v>11</v>
       </c>
       <c r="B22" s="3"/>
@@ -1735,7 +1724,7 @@
       <c r="P22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19" t="n">
+      <c r="A23" s="18" t="n">
         <v>12</v>
       </c>
       <c r="B23" s="3"/>
@@ -1755,7 +1744,7 @@
       <c r="P23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="n">
+      <c r="A24" s="18" t="n">
         <v>13</v>
       </c>
       <c r="B24" s="3"/>
@@ -1775,7 +1764,7 @@
       <c r="P24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19" t="n">
+      <c r="A25" s="18" t="n">
         <v>14</v>
       </c>
       <c r="B25" s="3"/>
@@ -1795,7 +1784,7 @@
       <c r="P25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="n">
+      <c r="A26" s="18" t="n">
         <v>15</v>
       </c>
       <c r="B26" s="3"/>
@@ -1815,7 +1804,7 @@
       <c r="P26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="n">
+      <c r="A27" s="18" t="n">
         <v>16</v>
       </c>
       <c r="B27" s="3"/>
@@ -1835,7 +1824,7 @@
       <c r="P27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="19" t="n">
+      <c r="A28" s="18" t="n">
         <v>17</v>
       </c>
       <c r="B28" s="3"/>
@@ -1855,7 +1844,7 @@
       <c r="P28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19" t="n">
+      <c r="A29" s="18" t="n">
         <v>18</v>
       </c>
       <c r="B29" s="3"/>
@@ -1875,7 +1864,7 @@
       <c r="P29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19" t="n">
+      <c r="A30" s="18" t="n">
         <v>19</v>
       </c>
       <c r="B30" s="3"/>
@@ -1895,7 +1884,7 @@
       <c r="P30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19" t="n">
+      <c r="A31" s="18" t="n">
         <v>20</v>
       </c>
       <c r="B31" s="3"/>
@@ -1915,7 +1904,7 @@
       <c r="P31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="19" t="n">
+      <c r="A32" s="18" t="n">
         <v>21</v>
       </c>
       <c r="B32" s="3"/>
@@ -1935,7 +1924,7 @@
       <c r="P32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="19" t="n">
+      <c r="A33" s="18" t="n">
         <v>22</v>
       </c>
       <c r="B33" s="3"/>
@@ -1955,7 +1944,7 @@
       <c r="P33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="19" t="n">
+      <c r="A34" s="18" t="n">
         <v>23</v>
       </c>
       <c r="B34" s="3"/>
@@ -1975,7 +1964,7 @@
       <c r="P34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="19" t="n">
+      <c r="A35" s="18" t="n">
         <v>24</v>
       </c>
       <c r="B35" s="3"/>
@@ -1995,7 +1984,7 @@
       <c r="P35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="19" t="n">
+      <c r="A36" s="18" t="n">
         <v>25</v>
       </c>
       <c r="B36" s="3"/>
@@ -2015,7 +2004,7 @@
       <c r="P36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="19" t="n">
+      <c r="A37" s="18" t="n">
         <v>26</v>
       </c>
       <c r="B37" s="3"/>
@@ -2035,7 +2024,7 @@
       <c r="P37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="19" t="n">
+      <c r="A38" s="18" t="n">
         <v>27</v>
       </c>
       <c r="B38" s="3"/>
@@ -2055,7 +2044,7 @@
       <c r="P38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19" t="n">
+      <c r="A39" s="18" t="n">
         <v>28</v>
       </c>
       <c r="B39" s="3"/>
@@ -2075,7 +2064,7 @@
       <c r="P39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="19" t="n">
+      <c r="A40" s="18" t="n">
         <v>29</v>
       </c>
       <c r="B40" s="3"/>
@@ -2095,12 +2084,12 @@
       <c r="P40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="19" t="n">
+      <c r="A41" s="18" t="n">
         <v>30</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -2115,12 +2104,12 @@
       <c r="P41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="19" t="n">
+      <c r="A42" s="18" t="n">
         <v>31</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -2135,12 +2124,12 @@
       <c r="P42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="19" t="n">
+      <c r="A43" s="18" t="n">
         <v>32</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -2155,12 +2144,12 @@
       <c r="P43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="19" t="n">
+      <c r="A44" s="18" t="n">
         <v>33</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -2175,12 +2164,12 @@
       <c r="P44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="19" t="n">
+      <c r="A45" s="18" t="n">
         <v>34</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -2195,12 +2184,12 @@
       <c r="P45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="19" t="n">
+      <c r="A46" s="18" t="n">
         <v>35</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -2215,12 +2204,12 @@
       <c r="P46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="19" t="n">
+      <c r="A47" s="18" t="n">
         <v>36</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -2235,12 +2224,12 @@
       <c r="P47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="19" t="n">
+      <c r="A48" s="18" t="n">
         <v>37</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -2255,12 +2244,12 @@
       <c r="P48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="19" t="n">
+      <c r="A49" s="18" t="n">
         <v>38</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -2275,12 +2264,12 @@
       <c r="P49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="19" t="n">
+      <c r="A50" s="18" t="n">
         <v>39</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -2295,12 +2284,12 @@
       <c r="P50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="19" t="n">
+      <c r="A51" s="18" t="n">
         <v>40</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -2315,12 +2304,12 @@
       <c r="P51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="19" t="n">
+      <c r="A52" s="18" t="n">
         <v>41</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -2335,12 +2324,12 @@
       <c r="P52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="19" t="n">
+      <c r="A53" s="18" t="n">
         <v>42</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -2355,12 +2344,12 @@
       <c r="P53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="19" t="n">
+      <c r="A54" s="18" t="n">
         <v>43</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -2375,12 +2364,12 @@
       <c r="P54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="19" t="n">
+      <c r="A55" s="18" t="n">
         <v>44</v>
       </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -2395,12 +2384,12 @@
       <c r="P55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="19" t="n">
+      <c r="A56" s="18" t="n">
         <v>45</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -2415,12 +2404,12 @@
       <c r="P56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="19" t="n">
+      <c r="A57" s="18" t="n">
         <v>46</v>
       </c>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -2435,12 +2424,12 @@
       <c r="P57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="19" t="n">
+      <c r="A58" s="18" t="n">
         <v>47</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -2455,12 +2444,12 @@
       <c r="P58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="19" t="n">
+      <c r="A59" s="18" t="n">
         <v>48</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -2475,12 +2464,12 @@
       <c r="P59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="19" t="n">
+      <c r="A60" s="18" t="n">
         <v>49</v>
       </c>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -2495,12 +2484,12 @@
       <c r="P60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="19" t="n">
+      <c r="A61" s="18" t="n">
         <v>50</v>
       </c>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -2515,12 +2504,12 @@
       <c r="P61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="19" t="n">
+      <c r="A62" s="18" t="n">
         <v>51</v>
       </c>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -2535,12 +2524,12 @@
       <c r="P62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="19" t="n">
+      <c r="A63" s="18" t="n">
         <v>52</v>
       </c>
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -2555,12 +2544,12 @@
       <c r="P63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="19" t="n">
+      <c r="A64" s="18" t="n">
         <v>53</v>
       </c>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -2575,12 +2564,12 @@
       <c r="P64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="19" t="n">
+      <c r="A65" s="18" t="n">
         <v>54</v>
       </c>
-      <c r="B65" s="21"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -2595,12 +2584,12 @@
       <c r="P65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="19" t="n">
+      <c r="A66" s="18" t="n">
         <v>55</v>
       </c>
-      <c r="B66" s="21"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -2615,12 +2604,12 @@
       <c r="P66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="19" t="n">
+      <c r="A67" s="18" t="n">
         <v>56</v>
       </c>
-      <c r="B67" s="21"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -2635,12 +2624,12 @@
       <c r="P67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="19" t="n">
+      <c r="A68" s="18" t="n">
         <v>57</v>
       </c>
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -2655,12 +2644,12 @@
       <c r="P68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="19" t="n">
+      <c r="A69" s="18" t="n">
         <v>58</v>
       </c>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -2675,12 +2664,12 @@
       <c r="P69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="19" t="n">
+      <c r="A70" s="18" t="n">
         <v>59</v>
       </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -2695,12 +2684,12 @@
       <c r="P70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="19" t="n">
+      <c r="A71" s="18" t="n">
         <v>60</v>
       </c>
-      <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -2715,12 +2704,12 @@
       <c r="P71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="19" t="n">
+      <c r="A72" s="18" t="n">
         <v>61</v>
       </c>
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -2735,12 +2724,12 @@
       <c r="P72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="19" t="n">
+      <c r="A73" s="18" t="n">
         <v>62</v>
       </c>
-      <c r="B73" s="21"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="20"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -2755,12 +2744,12 @@
       <c r="P73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="19" t="n">
+      <c r="A74" s="18" t="n">
         <v>63</v>
       </c>
-      <c r="B74" s="21"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
@@ -2775,12 +2764,12 @@
       <c r="P74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="19" t="n">
+      <c r="A75" s="18" t="n">
         <v>64</v>
       </c>
-      <c r="B75" s="21"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -2795,12 +2784,12 @@
       <c r="P75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="19" t="n">
+      <c r="A76" s="18" t="n">
         <v>65</v>
       </c>
-      <c r="B76" s="21"/>
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -2815,12 +2804,12 @@
       <c r="P76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="19" t="n">
+      <c r="A77" s="18" t="n">
         <v>66</v>
       </c>
-      <c r="B77" s="21"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="20"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -2835,12 +2824,12 @@
       <c r="P77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="19" t="n">
+      <c r="A78" s="18" t="n">
         <v>67</v>
       </c>
-      <c r="B78" s="21"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -2855,12 +2844,12 @@
       <c r="P78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="19" t="n">
+      <c r="A79" s="18" t="n">
         <v>68</v>
       </c>
-      <c r="B79" s="21"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -2875,12 +2864,12 @@
       <c r="P79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="19" t="n">
+      <c r="A80" s="18" t="n">
         <v>69</v>
       </c>
-      <c r="B80" s="21"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -2895,12 +2884,12 @@
       <c r="P80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="19" t="n">
+      <c r="A81" s="18" t="n">
         <v>70</v>
       </c>
-      <c r="B81" s="21"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -2915,12 +2904,12 @@
       <c r="P81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="19" t="n">
+      <c r="A82" s="18" t="n">
         <v>71</v>
       </c>
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -2935,12 +2924,12 @@
       <c r="P82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="19" t="n">
+      <c r="A83" s="18" t="n">
         <v>72</v>
       </c>
-      <c r="B83" s="21"/>
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
@@ -2955,12 +2944,12 @@
       <c r="P83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="19" t="n">
+      <c r="A84" s="18" t="n">
         <v>73</v>
       </c>
-      <c r="B84" s="21"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
@@ -2975,12 +2964,12 @@
       <c r="P84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="19" t="n">
+      <c r="A85" s="18" t="n">
         <v>74</v>
       </c>
-      <c r="B85" s="21"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="20"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -2995,12 +2984,12 @@
       <c r="P85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="19" t="n">
+      <c r="A86" s="18" t="n">
         <v>75</v>
       </c>
-      <c r="B86" s="21"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="21"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -3015,12 +3004,12 @@
       <c r="P86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="19" t="n">
+      <c r="A87" s="18" t="n">
         <v>76</v>
       </c>
-      <c r="B87" s="21"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="21"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -3035,12 +3024,12 @@
       <c r="P87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="19" t="n">
+      <c r="A88" s="18" t="n">
         <v>77</v>
       </c>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="20"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -3055,12 +3044,12 @@
       <c r="P88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="19" t="n">
+      <c r="A89" s="18" t="n">
         <v>78</v>
       </c>
-      <c r="B89" s="21"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="21"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -3075,12 +3064,12 @@
       <c r="P89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="19" t="n">
+      <c r="A90" s="18" t="n">
         <v>79</v>
       </c>
-      <c r="B90" s="21"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="21"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="20"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -3095,12 +3084,12 @@
       <c r="P90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="19" t="n">
+      <c r="A91" s="18" t="n">
         <v>80</v>
       </c>
-      <c r="B91" s="21"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="21"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="20"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -3115,12 +3104,12 @@
       <c r="P91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="19" t="n">
+      <c r="A92" s="18" t="n">
         <v>81</v>
       </c>
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="20"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
@@ -3135,12 +3124,12 @@
       <c r="P92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="19" t="n">
+      <c r="A93" s="18" t="n">
         <v>82</v>
       </c>
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="21"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="20"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -3155,12 +3144,12 @@
       <c r="P93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="19" t="n">
+      <c r="A94" s="18" t="n">
         <v>83</v>
       </c>
-      <c r="B94" s="21"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="21"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="20"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
@@ -3175,12 +3164,12 @@
       <c r="P94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="19" t="n">
+      <c r="A95" s="18" t="n">
         <v>84</v>
       </c>
-      <c r="B95" s="21"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="21"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="20"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
@@ -3195,12 +3184,12 @@
       <c r="P95" s="3"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="19" t="n">
+      <c r="A96" s="18" t="n">
         <v>85</v>
       </c>
-      <c r="B96" s="21"/>
-      <c r="C96" s="21"/>
-      <c r="D96" s="21"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="20"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
@@ -3215,12 +3204,12 @@
       <c r="P96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="19" t="n">
+      <c r="A97" s="18" t="n">
         <v>86</v>
       </c>
-      <c r="B97" s="21"/>
-      <c r="C97" s="21"/>
-      <c r="D97" s="21"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="20"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -3235,12 +3224,12 @@
       <c r="P97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="19" t="n">
+      <c r="A98" s="18" t="n">
         <v>87</v>
       </c>
-      <c r="B98" s="21"/>
-      <c r="C98" s="21"/>
-      <c r="D98" s="21"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="20"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
@@ -3255,12 +3244,12 @@
       <c r="P98" s="3"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="19" t="n">
+      <c r="A99" s="18" t="n">
         <v>88</v>
       </c>
-      <c r="B99" s="21"/>
-      <c r="C99" s="21"/>
-      <c r="D99" s="21"/>
+      <c r="B99" s="20"/>
+      <c r="C99" s="20"/>
+      <c r="D99" s="20"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
@@ -3275,12 +3264,12 @@
       <c r="P99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="19" t="n">
+      <c r="A100" s="18" t="n">
         <v>89</v>
       </c>
-      <c r="B100" s="21"/>
-      <c r="C100" s="21"/>
-      <c r="D100" s="21"/>
+      <c r="B100" s="20"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="20"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
@@ -3295,12 +3284,12 @@
       <c r="P100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="19" t="n">
+      <c r="A101" s="18" t="n">
         <v>90</v>
       </c>
-      <c r="B101" s="21"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="21"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
+      <c r="D101" s="20"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
@@ -3315,12 +3304,12 @@
       <c r="P101" s="3"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="19" t="n">
+      <c r="A102" s="18" t="n">
         <v>91</v>
       </c>
-      <c r="B102" s="21"/>
-      <c r="C102" s="21"/>
-      <c r="D102" s="21"/>
+      <c r="B102" s="20"/>
+      <c r="C102" s="20"/>
+      <c r="D102" s="20"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
@@ -3335,12 +3324,12 @@
       <c r="P102" s="3"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="19" t="n">
+      <c r="A103" s="18" t="n">
         <v>92</v>
       </c>
-      <c r="B103" s="21"/>
-      <c r="C103" s="21"/>
-      <c r="D103" s="21"/>
+      <c r="B103" s="20"/>
+      <c r="C103" s="20"/>
+      <c r="D103" s="20"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
@@ -3355,12 +3344,12 @@
       <c r="P103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="19" t="n">
+      <c r="A104" s="18" t="n">
         <v>93</v>
       </c>
-      <c r="B104" s="21"/>
-      <c r="C104" s="21"/>
-      <c r="D104" s="21"/>
+      <c r="B104" s="20"/>
+      <c r="C104" s="20"/>
+      <c r="D104" s="20"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
@@ -3375,12 +3364,12 @@
       <c r="P104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="19" t="n">
+      <c r="A105" s="18" t="n">
         <v>94</v>
       </c>
-      <c r="B105" s="21"/>
-      <c r="C105" s="21"/>
-      <c r="D105" s="21"/>
+      <c r="B105" s="20"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="20"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
@@ -3395,12 +3384,12 @@
       <c r="P105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="19" t="n">
+      <c r="A106" s="18" t="n">
         <v>95</v>
       </c>
-      <c r="B106" s="21"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="21"/>
+      <c r="B106" s="20"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="20"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -3415,12 +3404,12 @@
       <c r="P106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="19" t="n">
+      <c r="A107" s="18" t="n">
         <v>96</v>
       </c>
-      <c r="B107" s="21"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="21"/>
+      <c r="B107" s="20"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="20"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
@@ -3435,12 +3424,12 @@
       <c r="P107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="19" t="n">
+      <c r="A108" s="18" t="n">
         <v>97</v>
       </c>
-      <c r="B108" s="21"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="21"/>
+      <c r="B108" s="20"/>
+      <c r="C108" s="20"/>
+      <c r="D108" s="20"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
@@ -3455,12 +3444,12 @@
       <c r="P108" s="3"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="19" t="n">
+      <c r="A109" s="18" t="n">
         <v>98</v>
       </c>
-      <c r="B109" s="21"/>
-      <c r="C109" s="21"/>
-      <c r="D109" s="21"/>
+      <c r="B109" s="20"/>
+      <c r="C109" s="20"/>
+      <c r="D109" s="20"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
@@ -3475,12 +3464,12 @@
       <c r="P109" s="3"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="19" t="n">
+      <c r="A110" s="18" t="n">
         <v>99</v>
       </c>
-      <c r="B110" s="21"/>
-      <c r="C110" s="21"/>
-      <c r="D110" s="21"/>
+      <c r="B110" s="20"/>
+      <c r="C110" s="20"/>
+      <c r="D110" s="20"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
@@ -3495,7 +3484,7 @@
       <c r="P110" s="3"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="19" t="n">
+      <c r="A111" s="18" t="n">
         <v>100</v>
       </c>
       <c r="B111" s="3"/>
@@ -19702,7 +19691,7 @@
     <mergeCell ref="B8:P8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J11" r:id="rId1" display="https://agirpourlatransition.ademe.fr/entreprises/aides-financieres/2023/audit-energetique-industrie"/>
+    <hyperlink ref="J11" r:id="rId1" display="Lien permettant d'obtenir plus d'informations sur le dispositif. &#10;&#10;L'ajout d'un lien n'est pas obligatoire car certains dispositifs n'en disposent pas mais est très fortement recommandé&#10;&#10;Ex : https://agirpourlatransition.ademe.fr/entreprises/aides-financieres/2023/audit-energetique-industrie"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>